<commit_message>
upper bounds and other improvements
</commit_message>
<xml_diff>
--- a/fluxpersolarmass2.xlsx
+++ b/fluxpersolarmass2.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Desktop\Cluster folder for Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F674A435-1AF6-483C-966D-0B50F85BA249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D90D38-8718-4E1F-9A1C-8A8A94B922BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1DF6E311-3216-49A2-81DD-7F77491B3B49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$248</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="0">Sheet1!$Q$3:$Q$4</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -85,13 +89,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF0A0101"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,9 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +446,13 @@
   <dimension ref="A1:U248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q235" sqref="Q235"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -485,9 +500,7 @@
       <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="1">
-        <v>1.6971699999999999E-20</v>
-      </c>
+      <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -537,9 +550,8 @@
         <f>LOG10(M2/0.0207)</f>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U2" s="1">
-        <v>1.69996E-20</v>
-      </c>
+      <c r="R2" s="2"/>
+      <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -589,9 +601,7 @@
         <f t="shared" ref="O3:O66" si="1">LOG10(M3/0.0207)</f>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U3" s="1">
-        <v>2.2553399999999999E-20</v>
-      </c>
+      <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -641,9 +651,11 @@
         <f t="shared" si="1"/>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U4" s="1">
-        <v>2.9837799999999998E-20</v>
-      </c>
+      <c r="Q4" t="b">
+        <f>MOD(ROW(A2)-2,19)=0</f>
+        <v>1</v>
+      </c>
+      <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -693,9 +705,7 @@
         <f t="shared" si="1"/>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U5" s="1">
-        <v>3.66918E-20</v>
-      </c>
+      <c r="U5" s="1"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -745,9 +755,7 @@
         <f t="shared" si="1"/>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U6" s="1">
-        <v>5.8009799999999996E-20</v>
-      </c>
+      <c r="U6" s="1"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -797,9 +805,7 @@
         <f t="shared" si="1"/>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U7" s="1">
-        <v>8.8094300000000004E-20</v>
-      </c>
+      <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -849,9 +855,7 @@
         <f t="shared" si="1"/>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U8" s="1">
-        <v>1.1150100000000001E-19</v>
-      </c>
+      <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -901,9 +905,7 @@
         <f t="shared" si="1"/>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U9" s="1">
-        <v>7.2870400000000002E-20</v>
-      </c>
+      <c r="U9" s="1"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -953,9 +955,7 @@
         <f t="shared" si="1"/>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U10" s="1">
-        <v>2.7945200000000001E-20</v>
-      </c>
+      <c r="U10" s="1"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -1005,9 +1005,7 @@
         <f t="shared" si="1"/>
         <v>-2.6170003411208991</v>
       </c>
-      <c r="U11" s="1">
-        <v>1.50245E-20</v>
-      </c>
+      <c r="U11" s="1"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -12624,5 +12622,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>